<commit_message>
Added data - nothing major
</commit_message>
<xml_diff>
--- a/regression_summaries.xlsx
+++ b/regression_summaries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\shinycrab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{585D6E0F-D5A4-4652-834B-2B6B1907D445}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87403031-3B36-46B3-8C90-71C6A75826D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="270" windowWidth="19440" windowHeight="15000" xr2:uid="{92501DCD-C878-4E1C-B363-916EF62D2436}"/>
+    <workbookView xWindow="-19170" yWindow="420" windowWidth="18900" windowHeight="14730" xr2:uid="{92501DCD-C878-4E1C-B363-916EF62D2436}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="18">
   <si>
     <t>Independent</t>
   </si>
@@ -65,9 +65,6 @@
     <t>B90_SubAdultCPUE</t>
   </si>
   <si>
-    <t>Lag</t>
-  </si>
-  <si>
     <t>coef2</t>
   </si>
   <si>
@@ -81,6 +78,15 @@
   </si>
   <si>
     <t>B90_CPUE</t>
+  </si>
+  <si>
+    <t>IndependentGroup</t>
+  </si>
+  <si>
+    <t>Abundance</t>
+  </si>
+  <si>
+    <t>LagLead</t>
   </si>
 </sst>
 </file>
@@ -457,20 +463,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722DA1F2-E4C9-40C0-B65E-983E407382A3}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="11" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -478,335 +485,407 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.67971999999999999</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.46873999999999999</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>4.6E-6</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.47020000000000001</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.45557999999999998</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>32.83</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1.3569</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.30130000000000001</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>4.7210000000000004E-3</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.20130000000000001</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.17910000000000001</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>9.0739999999999998</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>1.7016</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.21859999999999999</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>4.7649999999999998E-2</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.1074</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>8.1939999999999999E-2</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>4.2130000000000001</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1.764</v>
+      </c>
+      <c r="F5">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="G5">
+        <v>4.7620000000000003E-2</v>
+      </c>
+      <c r="H5">
+        <v>0.1019</v>
+      </c>
+      <c r="I5">
+        <v>7.7619999999999995E-2</v>
+      </c>
+      <c r="J5">
+        <v>4.1980000000000004</v>
+      </c>
+      <c r="K5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
         <v>0</v>
       </c>
-      <c r="D5">
-        <v>1.764</v>
-      </c>
-      <c r="E5">
-        <v>0.22700000000000001</v>
-      </c>
-      <c r="F5">
-        <v>4.7620000000000003E-2</v>
-      </c>
-      <c r="G5">
-        <v>0.1019</v>
-      </c>
-      <c r="H5">
-        <v>7.7619999999999995E-2</v>
-      </c>
-      <c r="I5">
-        <v>4.1980000000000004</v>
-      </c>
-      <c r="J5">
+      <c r="E6">
+        <v>1.8703000000000001</v>
+      </c>
+      <c r="F6">
+        <v>0.24049999999999999</v>
+      </c>
+      <c r="G6">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="H6">
+        <v>8.3720000000000003E-2</v>
+      </c>
+      <c r="I6">
+        <v>5.8959999999999999E-2</v>
+      </c>
+      <c r="J6">
+        <v>3.3809999999999998</v>
+      </c>
+      <c r="K6">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C6">
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="D6">
-        <v>1.8703000000000001</v>
-      </c>
-      <c r="E6">
-        <v>0.24049999999999999</v>
-      </c>
-      <c r="F6">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="G6">
-        <v>8.3720000000000003E-2</v>
-      </c>
-      <c r="H6">
-        <v>5.8959999999999999E-2</v>
-      </c>
-      <c r="I6">
-        <v>3.3809999999999998</v>
-      </c>
-      <c r="J6">
+      <c r="E7" s="1">
+        <v>-3.2829999999999999E-3</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.73454799999999998</v>
+      </c>
+      <c r="G7" s="2">
+        <v>5.4770000000000003E-14</v>
+      </c>
+      <c r="H7">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="I7">
+        <v>0.78129999999999999</v>
+      </c>
+      <c r="J7">
+        <v>136.69999999999999</v>
+      </c>
+      <c r="K7">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1.5421</v>
+      </c>
+      <c r="F8">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="G8">
+        <v>3.0849999999999999E-2</v>
+      </c>
+      <c r="H8">
+        <v>0.123</v>
+      </c>
+      <c r="I8">
+        <v>9.8659999999999998E-2</v>
+      </c>
+      <c r="J8">
+        <v>5.05</v>
+      </c>
+      <c r="K8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>-3.2829999999999999E-3</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.73454799999999998</v>
-      </c>
-      <c r="F7" s="2">
-        <v>5.4770000000000003E-14</v>
-      </c>
-      <c r="G7">
-        <v>0.78700000000000003</v>
-      </c>
-      <c r="H7">
-        <v>0.78129999999999999</v>
-      </c>
-      <c r="I7">
-        <v>136.69999999999999</v>
-      </c>
-      <c r="J7">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1.5421</v>
-      </c>
-      <c r="E8">
-        <v>0.28499999999999998</v>
-      </c>
-      <c r="F8">
-        <v>3.0849999999999999E-2</v>
-      </c>
-      <c r="G8">
-        <v>0.123</v>
-      </c>
-      <c r="H8">
-        <v>9.8659999999999998E-2</v>
-      </c>
-      <c r="I8">
-        <v>5.05</v>
-      </c>
-      <c r="J8">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on listing regression relationships (E98 & T38Juv)
</commit_message>
<xml_diff>
--- a/regression_summaries.xlsx
+++ b/regression_summaries.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\shinycrab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7E273F-A917-4B4A-9768-E94C0A06D426}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62C15F9-8456-4FED-BD86-533F591A4962}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="270" windowWidth="19440" windowHeight="15000" xr2:uid="{92501DCD-C878-4E1C-B363-916EF62D2436}"/>
+    <workbookView xWindow="-19320" yWindow="270" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{92501DCD-C878-4E1C-B363-916EF62D2436}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="B90" sheetId="1" r:id="rId1"/>
+    <sheet name="E98" sheetId="2" r:id="rId2"/>
+    <sheet name="T38" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="101">
   <si>
     <t>Independent</t>
   </si>
@@ -270,6 +272,72 @@
   </si>
   <si>
     <t>ChasCity_MeanAnnualDailyPrecip</t>
+  </si>
+  <si>
+    <t>E98_JuvCPUE</t>
+  </si>
+  <si>
+    <t>E98_SubAdultCPUE</t>
+  </si>
+  <si>
+    <t>E98_AdultCPUE</t>
+  </si>
+  <si>
+    <t>E98_CPUE</t>
+  </si>
+  <si>
+    <t>AshleyLandingsCPUE</t>
+  </si>
+  <si>
+    <t>ENDED WITH SALINITY</t>
+  </si>
+  <si>
+    <t>T38_JuvCPUE</t>
+  </si>
+  <si>
+    <t>CustomsHouse_MeanAnnualTemp_WaterYr</t>
+  </si>
+  <si>
+    <t>ENSO_FM</t>
+  </si>
+  <si>
+    <t>ENSO_MA</t>
+  </si>
+  <si>
+    <t>ENSO_AM</t>
+  </si>
+  <si>
+    <t>ENSO_MJ</t>
+  </si>
+  <si>
+    <t>ENSO_JJ</t>
+  </si>
+  <si>
+    <t>ENSO_JA</t>
+  </si>
+  <si>
+    <t>ENSO</t>
+  </si>
+  <si>
+    <t>ONI_DJF</t>
+  </si>
+  <si>
+    <t>ONI_JFM</t>
+  </si>
+  <si>
+    <t>ONI_FMA</t>
+  </si>
+  <si>
+    <t>ONI_MAM</t>
+  </si>
+  <si>
+    <t>ONI_AMJ</t>
+  </si>
+  <si>
+    <t>ONI_MJJ</t>
+  </si>
+  <si>
+    <t>ONI_JJA</t>
   </si>
 </sst>
 </file>
@@ -626,9 +694,9 @@
   </sheetPr>
   <dimension ref="A1:K238"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A235" sqref="A235"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8974,4 +9042,2449 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4229D608-D66C-4CEF-BCC6-C7EEE69A9998}">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0.16807</v>
+      </c>
+      <c r="F2">
+        <v>0.23768</v>
+      </c>
+      <c r="G2">
+        <v>3.044E-12</v>
+      </c>
+      <c r="H2">
+        <v>0.93689999999999996</v>
+      </c>
+      <c r="I2">
+        <v>0.93340000000000001</v>
+      </c>
+      <c r="J2">
+        <v>267.10000000000002</v>
+      </c>
+      <c r="K2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>-1.4095200000000001</v>
+      </c>
+      <c r="F3">
+        <v>9.0986999999999998E-2</v>
+      </c>
+      <c r="G3">
+        <v>1.77E-8</v>
+      </c>
+      <c r="H3">
+        <v>0.83550000000000002</v>
+      </c>
+      <c r="I3">
+        <v>0.82640000000000002</v>
+      </c>
+      <c r="J3">
+        <v>91.44</v>
+      </c>
+      <c r="K3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>-0.19145000000000001</v>
+      </c>
+      <c r="F4">
+        <v>0.16273000000000001</v>
+      </c>
+      <c r="G4">
+        <v>1.8089999999999999E-13</v>
+      </c>
+      <c r="H4">
+        <v>0.95379999999999998</v>
+      </c>
+      <c r="I4">
+        <v>0.95130000000000003</v>
+      </c>
+      <c r="J4">
+        <v>371.8</v>
+      </c>
+      <c r="K4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>-4.0309999999999997</v>
+      </c>
+      <c r="F5">
+        <v>9.7520000000000001E-5</v>
+      </c>
+      <c r="G5">
+        <v>9.0969999999999995E-2</v>
+      </c>
+      <c r="H5">
+        <v>0.15049999999999999</v>
+      </c>
+      <c r="I5">
+        <v>0.1033</v>
+      </c>
+      <c r="J5">
+        <v>3.19</v>
+      </c>
+      <c r="K5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>-14.536</v>
+      </c>
+      <c r="F6">
+        <v>6.8879999999999999</v>
+      </c>
+      <c r="G6">
+        <v>7.9339999999999994E-2</v>
+      </c>
+      <c r="H6">
+        <v>0.218</v>
+      </c>
+      <c r="I6">
+        <v>0.1578</v>
+      </c>
+      <c r="J6">
+        <v>3.6240000000000001</v>
+      </c>
+      <c r="K6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>-22.187999999999999</v>
+      </c>
+      <c r="F7">
+        <v>2.2029999999999998</v>
+      </c>
+      <c r="G7">
+        <v>7.1679999999999994E-2</v>
+      </c>
+      <c r="H7">
+        <v>0.2283</v>
+      </c>
+      <c r="I7">
+        <v>0.16889999999999999</v>
+      </c>
+      <c r="J7">
+        <v>3.8450000000000002</v>
+      </c>
+      <c r="K7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>-22.187999999999999</v>
+      </c>
+      <c r="F8">
+        <v>8.81</v>
+      </c>
+      <c r="G8">
+        <v>7.1679999999999994E-2</v>
+      </c>
+      <c r="H8">
+        <v>0.2283</v>
+      </c>
+      <c r="I8">
+        <v>0.16889999999999999</v>
+      </c>
+      <c r="J8">
+        <v>3.8450000000000002</v>
+      </c>
+      <c r="K8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D18C0B-7C56-4AD9-89EB-B076C8DB8250}">
+  <dimension ref="A1:K62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>11.6433</v>
+      </c>
+      <c r="F2">
+        <v>-0.40189999999999998</v>
+      </c>
+      <c r="G2">
+        <v>6.3400000000000001E-3</v>
+      </c>
+      <c r="H2">
+        <v>0.22309999999999999</v>
+      </c>
+      <c r="I2">
+        <v>0.19719999999999999</v>
+      </c>
+      <c r="J2">
+        <v>8.6150000000000002</v>
+      </c>
+      <c r="K2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>12.599299999999999</v>
+      </c>
+      <c r="F3">
+        <v>-0.44040000000000001</v>
+      </c>
+      <c r="G3">
+        <v>2.8670000000000002E-3</v>
+      </c>
+      <c r="H3">
+        <v>0.26779999999999998</v>
+      </c>
+      <c r="I3">
+        <v>0.24260000000000001</v>
+      </c>
+      <c r="J3">
+        <v>10.61</v>
+      </c>
+      <c r="K3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3.4923700000000002</v>
+      </c>
+      <c r="F4">
+        <v>-0.16907</v>
+      </c>
+      <c r="G4">
+        <v>1.89E-2</v>
+      </c>
+      <c r="H4">
+        <v>0.43890000000000001</v>
+      </c>
+      <c r="I4">
+        <v>0.38279999999999997</v>
+      </c>
+      <c r="J4">
+        <v>7.8209999999999997</v>
+      </c>
+      <c r="K4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>11.9064</v>
+      </c>
+      <c r="F5">
+        <v>-0.4667</v>
+      </c>
+      <c r="G5">
+        <v>5.189E-3</v>
+      </c>
+      <c r="H5">
+        <v>0.34410000000000002</v>
+      </c>
+      <c r="I5">
+        <v>0.30959999999999999</v>
+      </c>
+      <c r="J5">
+        <v>9.968</v>
+      </c>
+      <c r="K5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0.98939999999999995</v>
+      </c>
+      <c r="F6">
+        <v>0.36840000000000001</v>
+      </c>
+      <c r="G6">
+        <v>6.8419999999999995E-2</v>
+      </c>
+      <c r="H6">
+        <v>0.29430000000000001</v>
+      </c>
+      <c r="I6">
+        <v>0.22370000000000001</v>
+      </c>
+      <c r="J6">
+        <v>4.17</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1.0542</v>
+      </c>
+      <c r="F7">
+        <v>0.46839999999999998</v>
+      </c>
+      <c r="G7">
+        <v>1.4189999999999999E-2</v>
+      </c>
+      <c r="H7">
+        <v>0.50539999999999996</v>
+      </c>
+      <c r="I7">
+        <v>0.45040000000000002</v>
+      </c>
+      <c r="J7">
+        <v>9.1950000000000003</v>
+      </c>
+      <c r="K7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1.0407</v>
+      </c>
+      <c r="F8">
+        <v>0.52810000000000001</v>
+      </c>
+      <c r="G8">
+        <v>6.1510000000000002E-3</v>
+      </c>
+      <c r="H8">
+        <v>0.58430000000000004</v>
+      </c>
+      <c r="I8">
+        <v>0.53810000000000002</v>
+      </c>
+      <c r="J8">
+        <v>12.65</v>
+      </c>
+      <c r="K8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>1.0766</v>
+      </c>
+      <c r="F9">
+        <v>0.50690000000000002</v>
+      </c>
+      <c r="G9">
+        <v>3.175E-2</v>
+      </c>
+      <c r="H9">
+        <v>0.45750000000000002</v>
+      </c>
+      <c r="I9">
+        <v>0.38969999999999999</v>
+      </c>
+      <c r="J9">
+        <v>6.7460000000000004</v>
+      </c>
+      <c r="K9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0.99050000000000005</v>
+      </c>
+      <c r="F10">
+        <v>0.43830000000000002</v>
+      </c>
+      <c r="G10">
+        <v>2.5489999999999999E-2</v>
+      </c>
+      <c r="H10">
+        <v>0.40749999999999997</v>
+      </c>
+      <c r="I10">
+        <v>0.34820000000000001</v>
+      </c>
+      <c r="J10">
+        <v>6.8780000000000001</v>
+      </c>
+      <c r="K10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>1.0804</v>
+      </c>
+      <c r="F11">
+        <v>0.48520000000000002</v>
+      </c>
+      <c r="G11">
+        <v>1.6619999999999999E-2</v>
+      </c>
+      <c r="H11">
+        <v>0.48909999999999998</v>
+      </c>
+      <c r="I11">
+        <v>0.43230000000000002</v>
+      </c>
+      <c r="J11">
+        <v>8.6150000000000002</v>
+      </c>
+      <c r="K11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0.99070000000000003</v>
+      </c>
+      <c r="F12">
+        <v>0.35549999999999998</v>
+      </c>
+      <c r="G12">
+        <v>6.9550000000000001E-2</v>
+      </c>
+      <c r="H12">
+        <v>0.2923</v>
+      </c>
+      <c r="I12">
+        <v>0.2215</v>
+      </c>
+      <c r="J12">
+        <v>4.13</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>1.044</v>
+      </c>
+      <c r="F13">
+        <v>0.33810000000000001</v>
+      </c>
+      <c r="G13">
+        <v>9.1560000000000002E-2</v>
+      </c>
+      <c r="H13">
+        <v>0.2838</v>
+      </c>
+      <c r="I13">
+        <v>0.20419999999999999</v>
+      </c>
+      <c r="J13">
+        <v>3.5659999999999998</v>
+      </c>
+      <c r="K13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1.6136999999999999</v>
+      </c>
+      <c r="F14">
+        <v>0.54849999999999999</v>
+      </c>
+      <c r="G14">
+        <v>3.026E-3</v>
+      </c>
+      <c r="H14">
+        <v>0.27350000000000002</v>
+      </c>
+      <c r="I14">
+        <v>0.2475</v>
+      </c>
+      <c r="J14">
+        <v>10.54</v>
+      </c>
+      <c r="K14">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1.591</v>
+      </c>
+      <c r="F15">
+        <v>0.59160000000000001</v>
+      </c>
+      <c r="G15">
+        <v>2.0790000000000001E-3</v>
+      </c>
+      <c r="H15">
+        <v>0.30049999999999999</v>
+      </c>
+      <c r="I15">
+        <v>0.27460000000000001</v>
+      </c>
+      <c r="J15">
+        <v>11.6</v>
+      </c>
+      <c r="K15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1.5608</v>
+      </c>
+      <c r="F16">
+        <v>0.59760000000000002</v>
+      </c>
+      <c r="G16">
+        <v>1.165E-3</v>
+      </c>
+      <c r="H16">
+        <v>0.3281</v>
+      </c>
+      <c r="I16">
+        <v>0.30320000000000003</v>
+      </c>
+      <c r="J16">
+        <v>13.18</v>
+      </c>
+      <c r="K16">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>1.5847</v>
+      </c>
+      <c r="F17">
+        <v>0.42749999999999999</v>
+      </c>
+      <c r="G17">
+        <v>3.1620000000000002E-2</v>
+      </c>
+      <c r="H17">
+        <v>0.1656</v>
+      </c>
+      <c r="I17">
+        <v>0.13350000000000001</v>
+      </c>
+      <c r="J17">
+        <v>5.16</v>
+      </c>
+      <c r="K17">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1.6327</v>
+      </c>
+      <c r="F18">
+        <v>0.5343</v>
+      </c>
+      <c r="G18">
+        <v>3.2039999999999998E-3</v>
+      </c>
+      <c r="H18">
+        <v>0.2626</v>
+      </c>
+      <c r="I18">
+        <v>0.23719999999999999</v>
+      </c>
+      <c r="J18">
+        <v>10.33</v>
+      </c>
+      <c r="K18">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>1.6191</v>
+      </c>
+      <c r="F19">
+        <v>0.44629999999999997</v>
+      </c>
+      <c r="G19">
+        <v>1.7919999999999998E-2</v>
+      </c>
+      <c r="H19">
+        <v>0.18429999999999999</v>
+      </c>
+      <c r="I19">
+        <v>0.15509999999999999</v>
+      </c>
+      <c r="J19">
+        <v>6.3259999999999996</v>
+      </c>
+      <c r="K19">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1.6327</v>
+      </c>
+      <c r="F20">
+        <v>0.40720000000000001</v>
+      </c>
+      <c r="G20">
+        <v>2.853E-2</v>
+      </c>
+      <c r="H20">
+        <v>0.15479999999999999</v>
+      </c>
+      <c r="I20">
+        <v>0.12570000000000001</v>
+      </c>
+      <c r="J20">
+        <v>5.3120000000000003</v>
+      </c>
+      <c r="K20">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>1.6134999999999999</v>
+      </c>
+      <c r="F21">
+        <v>0.34139999999999998</v>
+      </c>
+      <c r="G21">
+        <v>7.3410000000000003E-2</v>
+      </c>
+      <c r="H21">
+        <v>0.11</v>
+      </c>
+      <c r="I21">
+        <v>7.8189999999999996E-2</v>
+      </c>
+      <c r="J21">
+        <v>3.46</v>
+      </c>
+      <c r="K21">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1.4144000000000001</v>
+      </c>
+      <c r="F22">
+        <v>0.61650000000000005</v>
+      </c>
+      <c r="G22">
+        <v>3.3519999999999999E-3</v>
+      </c>
+      <c r="H22">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="I22">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="J22">
+        <v>11.41</v>
+      </c>
+      <c r="K22">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1.3432999999999999</v>
+      </c>
+      <c r="F23">
+        <v>0.61809999999999998</v>
+      </c>
+      <c r="G23">
+        <v>4.7449999999999999E-4</v>
+      </c>
+      <c r="H23">
+        <v>0.50170000000000003</v>
+      </c>
+      <c r="I23">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="J23">
+        <v>18.12</v>
+      </c>
+      <c r="K23">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>1.2444</v>
+      </c>
+      <c r="F24">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="G24">
+        <v>2.8559999999999999E-2</v>
+      </c>
+      <c r="H24">
+        <v>0.25190000000000001</v>
+      </c>
+      <c r="I24">
+        <v>0.20798</v>
+      </c>
+      <c r="J24">
+        <v>5.7240000000000002</v>
+      </c>
+      <c r="K24">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1.2952999999999999</v>
+      </c>
+      <c r="F25">
+        <v>0.65159999999999996</v>
+      </c>
+      <c r="G25">
+        <v>6.9090000000000004E-4</v>
+      </c>
+      <c r="H25">
+        <v>0.50160000000000005</v>
+      </c>
+      <c r="I25">
+        <v>0.47220000000000001</v>
+      </c>
+      <c r="J25">
+        <v>17.11</v>
+      </c>
+      <c r="K25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1.2474000000000001</v>
+      </c>
+      <c r="F26">
+        <v>0.5252</v>
+      </c>
+      <c r="G26">
+        <v>3.9150000000000001E-3</v>
+      </c>
+      <c r="H26">
+        <v>0.39560000000000001</v>
+      </c>
+      <c r="I26">
+        <v>0.36009999999999998</v>
+      </c>
+      <c r="J26">
+        <v>11.13</v>
+      </c>
+      <c r="K26">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1.4151</v>
+      </c>
+      <c r="F27">
+        <v>0.55310000000000004</v>
+      </c>
+      <c r="G27">
+        <v>1.337E-2</v>
+      </c>
+      <c r="H27">
+        <v>0.29480000000000001</v>
+      </c>
+      <c r="I27">
+        <v>0.25559999999999999</v>
+      </c>
+      <c r="J27">
+        <v>7.5229999999999997</v>
+      </c>
+      <c r="K27">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1.3441000000000001</v>
+      </c>
+      <c r="F28">
+        <v>0.62829999999999997</v>
+      </c>
+      <c r="G28">
+        <v>5.9829999999999996E-4</v>
+      </c>
+      <c r="H28">
+        <v>0.48930000000000001</v>
+      </c>
+      <c r="I28">
+        <v>0.46089999999999998</v>
+      </c>
+      <c r="J28">
+        <v>17.239999999999998</v>
+      </c>
+      <c r="K28">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>1.2521</v>
+      </c>
+      <c r="F29">
+        <v>0.37819999999999998</v>
+      </c>
+      <c r="G29">
+        <v>3.8859999999999999E-2</v>
+      </c>
+      <c r="H29">
+        <v>0.2276</v>
+      </c>
+      <c r="I29">
+        <v>0.1822</v>
+      </c>
+      <c r="J29">
+        <v>5.0110000000000001</v>
+      </c>
+      <c r="K29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1.2958000000000001</v>
+      </c>
+      <c r="F30">
+        <v>0.58289999999999997</v>
+      </c>
+      <c r="G30">
+        <v>4.9719999999999999E-3</v>
+      </c>
+      <c r="H30">
+        <v>0.37959999999999999</v>
+      </c>
+      <c r="I30">
+        <v>0.34310000000000002</v>
+      </c>
+      <c r="J30">
+        <v>10.4</v>
+      </c>
+      <c r="K30">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1.2479</v>
+      </c>
+      <c r="F31">
+        <v>0.54369999999999996</v>
+      </c>
+      <c r="G31">
+        <v>3.6110000000000001E-3</v>
+      </c>
+      <c r="H31">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="I31">
+        <v>0.36570000000000003</v>
+      </c>
+      <c r="J31">
+        <v>11.38</v>
+      </c>
+      <c r="K31">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>4.2662000000000004</v>
+      </c>
+      <c r="F32">
+        <v>-0.10782</v>
+      </c>
+      <c r="G32">
+        <v>9.0529999999999999E-2</v>
+      </c>
+      <c r="H32">
+        <v>7.5480000000000005E-2</v>
+      </c>
+      <c r="I32">
+        <v>5.049E-2</v>
+      </c>
+      <c r="J32">
+        <v>3.0209999999999999</v>
+      </c>
+      <c r="K32">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>4.4584999999999999</v>
+      </c>
+      <c r="F33">
+        <v>-0.1129</v>
+      </c>
+      <c r="G33">
+        <v>9.7809999999999994E-2</v>
+      </c>
+      <c r="H33">
+        <v>7.6359999999999997E-2</v>
+      </c>
+      <c r="I33">
+        <v>4.9970000000000001E-2</v>
+      </c>
+      <c r="J33">
+        <v>2.8929999999999998</v>
+      </c>
+      <c r="K33">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>3.2880400000000001</v>
+      </c>
+      <c r="F34">
+        <v>-0.10861999999999999</v>
+      </c>
+      <c r="G34">
+        <v>4.3049999999999998E-2</v>
+      </c>
+      <c r="H34">
+        <v>0.2989</v>
+      </c>
+      <c r="I34">
+        <v>0.24049999999999999</v>
+      </c>
+      <c r="J34">
+        <v>5.117</v>
+      </c>
+      <c r="K34">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>5.55783</v>
+      </c>
+      <c r="F35">
+        <v>-0.19811999999999999</v>
+      </c>
+      <c r="G35">
+        <v>4.845E-2</v>
+      </c>
+      <c r="H35">
+        <v>0.3664</v>
+      </c>
+      <c r="I35">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="J35">
+        <v>5.2050000000000001</v>
+      </c>
+      <c r="K35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>-9.0135000000000005</v>
+      </c>
+      <c r="F36">
+        <v>0.50560000000000005</v>
+      </c>
+      <c r="G36">
+        <v>3.5839999999999997E-2</v>
+      </c>
+      <c r="H36">
+        <v>0.2117</v>
+      </c>
+      <c r="I36">
+        <v>0.17019999999999999</v>
+      </c>
+      <c r="J36">
+        <v>5.1020000000000003</v>
+      </c>
+      <c r="K36">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>12.7202</v>
+      </c>
+      <c r="F37">
+        <v>-0.54449999999999998</v>
+      </c>
+      <c r="G37">
+        <v>3.6490000000000002E-2</v>
+      </c>
+      <c r="H37">
+        <v>0.192</v>
+      </c>
+      <c r="I37">
+        <v>0.1535</v>
+      </c>
+      <c r="J37">
+        <v>4.9909999999999997</v>
+      </c>
+      <c r="K37">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <v>11.692</v>
+      </c>
+      <c r="F38">
+        <v>-0.50209999999999999</v>
+      </c>
+      <c r="G38">
+        <v>5.713E-2</v>
+      </c>
+      <c r="H38">
+        <v>0.17749999999999999</v>
+      </c>
+      <c r="I38">
+        <v>0.1343</v>
+      </c>
+      <c r="J38">
+        <v>4.101</v>
+      </c>
+      <c r="K38">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>8.8087999999999997</v>
+      </c>
+      <c r="F39">
+        <v>-0.35830000000000001</v>
+      </c>
+      <c r="G39">
+        <v>1.311E-2</v>
+      </c>
+      <c r="H39">
+        <v>0.41360000000000002</v>
+      </c>
+      <c r="I39">
+        <v>0.36470000000000002</v>
+      </c>
+      <c r="J39">
+        <v>8.4619999999999997</v>
+      </c>
+      <c r="K39">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <v>0.83028000000000002</v>
+      </c>
+      <c r="F40">
+        <v>7.0949999999999999E-2</v>
+      </c>
+      <c r="G40">
+        <v>3.6510000000000001E-2</v>
+      </c>
+      <c r="H40">
+        <v>0.1129</v>
+      </c>
+      <c r="I40">
+        <v>8.8910000000000003E-2</v>
+      </c>
+      <c r="J40">
+        <v>4.7080000000000002</v>
+      </c>
+      <c r="K40">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>1.6264000000000001</v>
+      </c>
+      <c r="F41">
+        <v>0.39660000000000001</v>
+      </c>
+      <c r="G41">
+        <v>2.545E-2</v>
+      </c>
+      <c r="H41">
+        <v>0.1278</v>
+      </c>
+      <c r="I41">
+        <v>0.1042</v>
+      </c>
+      <c r="J41">
+        <v>5.4219999999999997</v>
+      </c>
+      <c r="K41">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1.6294999999999999</v>
+      </c>
+      <c r="F42">
+        <v>0.38250000000000001</v>
+      </c>
+      <c r="G42">
+        <v>3.1649999999999998E-2</v>
+      </c>
+      <c r="H42">
+        <v>0.1188</v>
+      </c>
+      <c r="I42">
+        <v>9.4990000000000005E-2</v>
+      </c>
+      <c r="J42">
+        <v>4.9889999999999999</v>
+      </c>
+      <c r="K42">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>1.6313</v>
+      </c>
+      <c r="F43">
+        <v>0.41310000000000002</v>
+      </c>
+      <c r="G43">
+        <v>2.0049999999999998E-2</v>
+      </c>
+      <c r="H43">
+        <v>0.13769999999999999</v>
+      </c>
+      <c r="I43">
+        <v>0.1144</v>
+      </c>
+      <c r="J43">
+        <v>5.907</v>
+      </c>
+      <c r="K43">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>1.621</v>
+      </c>
+      <c r="F44">
+        <v>0.47660000000000002</v>
+      </c>
+      <c r="G44">
+        <v>7.4050000000000001E-3</v>
+      </c>
+      <c r="H44">
+        <v>0.17829999999999999</v>
+      </c>
+      <c r="I44">
+        <v>0.15609999999999999</v>
+      </c>
+      <c r="J44">
+        <v>8.0310000000000006</v>
+      </c>
+      <c r="K44">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1.6264000000000001</v>
+      </c>
+      <c r="F45">
+        <v>0.42609999999999998</v>
+      </c>
+      <c r="G45">
+        <v>1.6299999999999999E-2</v>
+      </c>
+      <c r="H45">
+        <v>0.1462</v>
+      </c>
+      <c r="I45">
+        <v>0.1231</v>
+      </c>
+      <c r="J45">
+        <v>6.335</v>
+      </c>
+      <c r="K45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>1.6424000000000001</v>
+      </c>
+      <c r="F46">
+        <v>0.3342</v>
+      </c>
+      <c r="G46">
+        <v>6.6739999999999994E-2</v>
+      </c>
+      <c r="H46">
+        <v>9.0329999999999994E-2</v>
+      </c>
+      <c r="I46">
+        <v>6.5060000000000007E-2</v>
+      </c>
+      <c r="J46">
+        <v>3.5750000000000002</v>
+      </c>
+      <c r="K46">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>1.6358999999999999</v>
+      </c>
+      <c r="F47">
+        <v>0.29609999999999997</v>
+      </c>
+      <c r="G47">
+        <v>9.9790000000000004E-2</v>
+      </c>
+      <c r="H47">
+        <v>7.152E-2</v>
+      </c>
+      <c r="I47">
+        <v>4.6420000000000003E-2</v>
+      </c>
+      <c r="J47">
+        <v>2.85</v>
+      </c>
+      <c r="K47">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" t="s">
+        <v>68</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>1.6425000000000001</v>
+      </c>
+      <c r="F48">
+        <v>0.46920000000000001</v>
+      </c>
+      <c r="G48">
+        <v>7.9349999999999993E-3</v>
+      </c>
+      <c r="H48">
+        <v>0.18</v>
+      </c>
+      <c r="I48">
+        <v>0.15720000000000001</v>
+      </c>
+      <c r="J48">
+        <v>7.9029999999999996</v>
+      </c>
+      <c r="K48">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" t="s">
+        <v>68</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49">
+        <v>1.6426000000000001</v>
+      </c>
+      <c r="F49">
+        <v>0.43619999999999998</v>
+      </c>
+      <c r="G49">
+        <v>1.4460000000000001E-2</v>
+      </c>
+      <c r="H49">
+        <v>0.155</v>
+      </c>
+      <c r="I49">
+        <v>0.13150000000000001</v>
+      </c>
+      <c r="J49">
+        <v>6.6050000000000004</v>
+      </c>
+      <c r="K49">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>92</v>
+      </c>
+      <c r="C50" t="s">
+        <v>68</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <v>1.6423000000000001</v>
+      </c>
+      <c r="F50">
+        <v>0.39250000000000002</v>
+      </c>
+      <c r="G50">
+        <v>2.9250000000000002E-2</v>
+      </c>
+      <c r="H50">
+        <v>0.12529999999999999</v>
+      </c>
+      <c r="I50">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="J50">
+        <v>5.1559999999999997</v>
+      </c>
+      <c r="K50">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>69</v>
+      </c>
+      <c r="C51" t="s">
+        <v>68</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="E51">
+        <v>1.6426000000000001</v>
+      </c>
+      <c r="F51">
+        <v>0.49009999999999998</v>
+      </c>
+      <c r="G51">
+        <v>5.6100000000000004E-3</v>
+      </c>
+      <c r="H51">
+        <v>0.1943</v>
+      </c>
+      <c r="I51">
+        <v>0.1719</v>
+      </c>
+      <c r="J51">
+        <v>8.6809999999999992</v>
+      </c>
+      <c r="K51">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>1.645</v>
+      </c>
+      <c r="F52">
+        <v>0.51790000000000003</v>
+      </c>
+      <c r="G52">
+        <v>3.1050000000000001E-3</v>
+      </c>
+      <c r="H52">
+        <v>0.21829999999999999</v>
+      </c>
+      <c r="I52">
+        <v>0.19650000000000001</v>
+      </c>
+      <c r="J52">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="K52">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" t="s">
+        <v>68</v>
+      </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
+      <c r="E53">
+        <v>1.6412</v>
+      </c>
+      <c r="F53">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="G53">
+        <v>1.1129999999999999E-2</v>
+      </c>
+      <c r="H53">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="I53">
+        <v>0.14280000000000001</v>
+      </c>
+      <c r="J53">
+        <v>7.1639999999999997</v>
+      </c>
+      <c r="K53">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>72</v>
+      </c>
+      <c r="C54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54">
+        <v>1.6367</v>
+      </c>
+      <c r="F54">
+        <v>0.42949999999999999</v>
+      </c>
+      <c r="G54">
+        <v>1.5689999999999999E-2</v>
+      </c>
+      <c r="H54">
+        <v>0.15160000000000001</v>
+      </c>
+      <c r="I54">
+        <v>0.128</v>
+      </c>
+      <c r="J54">
+        <v>6.4320000000000004</v>
+      </c>
+      <c r="K54">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>93</v>
+      </c>
+      <c r="C55" t="s">
+        <v>68</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>1.6324000000000001</v>
+      </c>
+      <c r="F55">
+        <v>0.68159999999999998</v>
+      </c>
+      <c r="G55">
+        <v>4.9420000000000002E-3</v>
+      </c>
+      <c r="H55">
+        <v>0.19950000000000001</v>
+      </c>
+      <c r="I55">
+        <v>0.1772</v>
+      </c>
+      <c r="J55">
+        <v>8.9700000000000006</v>
+      </c>
+      <c r="K55">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" t="s">
+        <v>68</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>1.6244000000000001</v>
+      </c>
+      <c r="F56">
+        <v>0.3543</v>
+      </c>
+      <c r="G56">
+        <v>2.9309999999999999E-2</v>
+      </c>
+      <c r="H56">
+        <v>0.122</v>
+      </c>
+      <c r="I56">
+        <v>9.8239999999999994E-2</v>
+      </c>
+      <c r="J56">
+        <v>5.14</v>
+      </c>
+      <c r="K56">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>95</v>
+      </c>
+      <c r="C57" t="s">
+        <v>68</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1.6201000000000001</v>
+      </c>
+      <c r="F57">
+        <v>0.36859999999999998</v>
+      </c>
+      <c r="G57">
+        <v>5.4199999999999998E-2</v>
+      </c>
+      <c r="H57">
+        <v>9.6549999999999997E-2</v>
+      </c>
+      <c r="I57">
+        <v>7.213E-2</v>
+      </c>
+      <c r="J57">
+        <v>3.9540000000000002</v>
+      </c>
+      <c r="K57">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>96</v>
+      </c>
+      <c r="C58" t="s">
+        <v>68</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>1.6136999999999999</v>
+      </c>
+      <c r="F58">
+        <v>0.44750000000000001</v>
+      </c>
+      <c r="G58">
+        <v>6.2280000000000002E-2</v>
+      </c>
+      <c r="H58">
+        <v>9.0810000000000002E-2</v>
+      </c>
+      <c r="I58">
+        <v>6.6239999999999993E-2</v>
+      </c>
+      <c r="J58">
+        <v>3.6960000000000002</v>
+      </c>
+      <c r="K58">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" t="s">
+        <v>68</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59">
+        <v>1.5999000000000001</v>
+      </c>
+      <c r="F59">
+        <v>0.58530000000000004</v>
+      </c>
+      <c r="G59">
+        <v>4.8090000000000001E-2</v>
+      </c>
+      <c r="H59">
+        <v>0.10150000000000001</v>
+      </c>
+      <c r="I59">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="J59">
+        <v>4.1790000000000003</v>
+      </c>
+      <c r="K59">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>98</v>
+      </c>
+      <c r="C60" t="s">
+        <v>68</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60">
+        <v>1.591</v>
+      </c>
+      <c r="F60">
+        <v>0.77859999999999996</v>
+      </c>
+      <c r="G60">
+        <v>9.9010000000000001E-3</v>
+      </c>
+      <c r="H60">
+        <v>0.1666</v>
+      </c>
+      <c r="I60">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="J60">
+        <v>7.3949999999999996</v>
+      </c>
+      <c r="K60">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>99</v>
+      </c>
+      <c r="C61" t="s">
+        <v>68</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>1.5958000000000001</v>
+      </c>
+      <c r="F61">
+        <v>0.8014</v>
+      </c>
+      <c r="G61">
+        <v>7.5880000000000001E-3</v>
+      </c>
+      <c r="H61">
+        <v>0.1774</v>
+      </c>
+      <c r="I61">
+        <v>0.15509999999999999</v>
+      </c>
+      <c r="J61">
+        <v>7.9770000000000003</v>
+      </c>
+      <c r="K61">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>100</v>
+      </c>
+      <c r="C62" t="s">
+        <v>68</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>1.6176999999999999</v>
+      </c>
+      <c r="F62">
+        <v>0.63859999999999995</v>
+      </c>
+      <c r="G62">
+        <v>1.5679999999999999E-2</v>
+      </c>
+      <c r="H62">
+        <v>0.14779999999999999</v>
+      </c>
+      <c r="I62">
+        <v>0.12479999999999999</v>
+      </c>
+      <c r="J62">
+        <v>6.4160000000000004</v>
+      </c>
+      <c r="K62">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Worked on landings ~ abiotics summary
</commit_message>
<xml_diff>
--- a/regression_summaries.xlsx
+++ b/regression_summaries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sczwa\Desktop\shinycrab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4102D795-0940-4803-9172-A03D97CA6D7F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C24D3E6-D7FA-423E-A9A5-2972410B4BBA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4095" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="7" xr2:uid="{92501DCD-C878-4E1C-B363-916EF62D2436}"/>
+    <workbookView xWindow="20370" yWindow="-4095" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="3" xr2:uid="{92501DCD-C878-4E1C-B363-916EF62D2436}"/>
   </bookViews>
   <sheets>
     <sheet name="E98" sheetId="2" r:id="rId1"/>
@@ -10128,9 +10128,9 @@
   </sheetPr>
   <dimension ref="A1:K124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B4:H20"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10247,7 +10247,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -10282,39 +10282,39 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>-91.662999999999997</v>
+        <v>6.28</v>
       </c>
       <c r="F5">
-        <v>4.6040000000000001</v>
+        <v>3.0150000000000001</v>
       </c>
       <c r="G5">
-        <v>6.4269999999999994E-2</v>
+        <v>1.748E-3</v>
       </c>
       <c r="H5">
-        <v>0.2777</v>
+        <v>0.64129999999999998</v>
       </c>
       <c r="I5">
-        <v>0.21199999999999999</v>
+        <v>0.60540000000000005</v>
       </c>
       <c r="J5">
-        <v>4.2290000000000001</v>
+        <v>17.88</v>
       </c>
       <c r="K5">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -10352,7 +10352,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -10527,7 +10527,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -10597,47 +10597,47 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>-35.856999999999999</v>
+        <v>5.9633000000000003</v>
       </c>
       <c r="F14">
-        <v>2.2240000000000002</v>
+        <v>2.9809999999999999</v>
       </c>
       <c r="G14">
-        <v>7.2859999999999994E-2</v>
+        <v>6.8900000000000003E-3</v>
       </c>
       <c r="H14">
-        <v>8.9020000000000002E-2</v>
+        <v>0.57430000000000003</v>
       </c>
       <c r="I14">
-        <v>6.2990000000000004E-2</v>
+        <v>0.52700000000000002</v>
       </c>
       <c r="J14">
-        <v>3.42</v>
+        <v>12.14</v>
       </c>
       <c r="K14">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
@@ -10646,25 +10646,25 @@
         <v>1</v>
       </c>
       <c r="E15">
-        <v>6.28</v>
+        <v>8.8879999999999999</v>
       </c>
       <c r="F15">
-        <v>3.0150000000000001</v>
+        <v>3.899</v>
       </c>
       <c r="G15">
-        <v>1.748E-3</v>
+        <v>1.1509999999999999E-2</v>
       </c>
       <c r="H15">
-        <v>0.64129999999999998</v>
+        <v>0.32050000000000001</v>
       </c>
       <c r="I15">
-        <v>0.60540000000000005</v>
+        <v>0.28060000000000002</v>
       </c>
       <c r="J15">
-        <v>17.88</v>
+        <v>8.02</v>
       </c>
       <c r="K15">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -10702,7 +10702,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -10772,12 +10772,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
@@ -10786,28 +10786,28 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <v>5.9633000000000003</v>
+        <v>6.2613000000000003</v>
       </c>
       <c r="F19">
-        <v>2.9809999999999999</v>
+        <v>2.2818999999999998</v>
       </c>
       <c r="G19">
-        <v>6.8900000000000003E-3</v>
+        <v>4.4880000000000003E-2</v>
       </c>
       <c r="H19">
-        <v>0.57430000000000003</v>
+        <v>0.34439999999999998</v>
       </c>
       <c r="I19">
-        <v>0.52700000000000002</v>
+        <v>0.27879999999999999</v>
       </c>
       <c r="J19">
-        <v>12.14</v>
+        <v>5.2519999999999998</v>
       </c>
       <c r="K19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -10877,7 +10877,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -11087,7 +11087,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -11122,7 +11122,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -11157,7 +11157,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -11227,7 +11227,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -11262,7 +11262,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -11402,47 +11402,47 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C37" t="s">
         <v>38</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E37">
-        <v>8.8879999999999999</v>
+        <v>6.1440000000000001</v>
       </c>
       <c r="F37">
-        <v>3.899</v>
+        <v>2.298</v>
       </c>
       <c r="G37">
-        <v>1.1509999999999999E-2</v>
+        <v>6.4509999999999998E-2</v>
       </c>
       <c r="H37">
-        <v>0.32050000000000001</v>
+        <v>0.3301</v>
       </c>
       <c r="I37">
-        <v>0.28060000000000002</v>
+        <v>0.25559999999999999</v>
       </c>
       <c r="J37">
-        <v>8.02</v>
+        <v>4.4340000000000002</v>
       </c>
       <c r="K37">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>14</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C38" t="s">
         <v>38</v>
@@ -11451,28 +11451,28 @@
         <v>1</v>
       </c>
       <c r="E38">
-        <v>6.2613000000000003</v>
+        <v>8.7409999999999997</v>
       </c>
       <c r="F38">
-        <v>2.2818999999999998</v>
+        <v>3.427</v>
       </c>
       <c r="G38">
-        <v>4.4880000000000003E-2</v>
+        <v>1.453E-2</v>
       </c>
       <c r="H38">
-        <v>0.34439999999999998</v>
+        <v>0.28889999999999999</v>
       </c>
       <c r="I38">
-        <v>0.27879999999999999</v>
+        <v>0.24940000000000001</v>
       </c>
       <c r="J38">
-        <v>5.2519999999999998</v>
+        <v>7.3109999999999999</v>
       </c>
       <c r="K38">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -11647,7 +11647,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>24</v>
       </c>
@@ -11682,39 +11682,39 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>14</v>
       </c>
       <c r="B45" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C45" t="s">
         <v>38</v>
       </c>
       <c r="D45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E45">
-        <v>6.1440000000000001</v>
+        <v>8.8840000000000003</v>
       </c>
       <c r="F45">
-        <v>2.298</v>
+        <v>3.516</v>
       </c>
       <c r="G45">
-        <v>6.4509999999999998E-2</v>
+        <v>2.0959999999999999E-2</v>
       </c>
       <c r="H45">
-        <v>0.3301</v>
+        <v>0.27579999999999999</v>
       </c>
       <c r="I45">
-        <v>0.25559999999999999</v>
+        <v>0.23319999999999999</v>
       </c>
       <c r="J45">
-        <v>4.4340000000000002</v>
+        <v>6.4729999999999999</v>
       </c>
       <c r="K45">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -11752,39 +11752,39 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C47" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>8.7409999999999997</v>
+        <v>-91.662999999999997</v>
       </c>
       <c r="F47">
-        <v>3.427</v>
+        <v>4.6040000000000001</v>
       </c>
       <c r="G47">
-        <v>1.453E-2</v>
+        <v>6.4269999999999994E-2</v>
       </c>
       <c r="H47">
-        <v>0.28889999999999999</v>
+        <v>0.2777</v>
       </c>
       <c r="I47">
-        <v>0.24940000000000001</v>
+        <v>0.21199999999999999</v>
       </c>
       <c r="J47">
-        <v>7.3109999999999999</v>
+        <v>4.2290000000000001</v>
       </c>
       <c r="K47">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -11892,39 +11892,39 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>14</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C51" t="s">
         <v>38</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E51">
-        <v>8.8840000000000003</v>
+        <v>17.6508</v>
       </c>
       <c r="F51">
-        <v>3.516</v>
+        <v>-0.77590000000000003</v>
       </c>
       <c r="G51">
-        <v>2.0959999999999999E-2</v>
+        <v>7.5660000000000005E-2</v>
       </c>
       <c r="H51">
-        <v>0.27579999999999999</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="I51">
-        <v>0.23319999999999999</v>
+        <v>0.2102</v>
       </c>
       <c r="J51">
-        <v>6.4729999999999999</v>
+        <v>3.927</v>
       </c>
       <c r="K51">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -12067,12 +12067,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>14</v>
       </c>
       <c r="B56" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C56" t="s">
         <v>38</v>
@@ -12081,25 +12081,25 @@
         <v>2</v>
       </c>
       <c r="E56">
-        <v>17.6508</v>
+        <v>83923</v>
       </c>
       <c r="F56">
-        <v>-0.77590000000000003</v>
+        <v>3.3450000000000002</v>
       </c>
       <c r="G56">
-        <v>7.5660000000000005E-2</v>
+        <v>3.5970000000000002E-2</v>
       </c>
       <c r="H56">
-        <v>0.28199999999999997</v>
+        <v>0.24679999999999999</v>
       </c>
       <c r="I56">
-        <v>0.2102</v>
+        <v>0.19969999999999999</v>
       </c>
       <c r="J56">
-        <v>3.927</v>
+        <v>5.242</v>
       </c>
       <c r="K56">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -12137,12 +12137,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>14</v>
       </c>
       <c r="B58" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C58" t="s">
         <v>38</v>
@@ -12151,22 +12151,22 @@
         <v>2</v>
       </c>
       <c r="E58">
-        <v>83923</v>
+        <v>8.84</v>
       </c>
       <c r="F58">
-        <v>3.3450000000000002</v>
+        <v>3.3860000000000001</v>
       </c>
       <c r="G58">
-        <v>3.5970000000000002E-2</v>
+        <v>3.8420000000000003E-2</v>
       </c>
       <c r="H58">
-        <v>0.24679999999999999</v>
+        <v>0.24129999999999999</v>
       </c>
       <c r="I58">
-        <v>0.19969999999999999</v>
+        <v>0.19389999999999999</v>
       </c>
       <c r="J58">
-        <v>5.242</v>
+        <v>5.09</v>
       </c>
       <c r="K58">
         <v>16</v>
@@ -12207,42 +12207,42 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>14</v>
       </c>
       <c r="B60" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C60" t="s">
         <v>38</v>
       </c>
       <c r="D60">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E60">
-        <v>8.84</v>
+        <v>8.6539999999999999</v>
       </c>
       <c r="F60">
-        <v>3.3860000000000001</v>
+        <v>3.1080000000000001</v>
       </c>
       <c r="G60">
-        <v>3.8420000000000003E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="H60">
-        <v>0.24129999999999999</v>
+        <v>0.2142</v>
       </c>
       <c r="I60">
-        <v>0.19389999999999999</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="J60">
-        <v>5.09</v>
+        <v>4.6340000000000003</v>
       </c>
       <c r="K60">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>24</v>
       </c>
@@ -12382,7 +12382,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -12417,39 +12417,39 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>14</v>
       </c>
       <c r="B66" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C66" t="s">
         <v>38</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66">
-        <v>8.6539999999999999</v>
+        <v>9.5139999999999993</v>
       </c>
       <c r="F66">
-        <v>3.1080000000000001</v>
+        <v>2.794</v>
       </c>
       <c r="G66">
-        <v>4.5999999999999999E-2</v>
+        <v>1.555E-2</v>
       </c>
       <c r="H66">
-        <v>0.2142</v>
+        <v>0.19159999999999999</v>
       </c>
       <c r="I66">
-        <v>0.16800000000000001</v>
+        <v>0.1628</v>
       </c>
       <c r="J66">
-        <v>4.6340000000000003</v>
+        <v>6.6379999999999999</v>
       </c>
       <c r="K66">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -12522,12 +12522,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>14</v>
       </c>
       <c r="B69" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C69" t="s">
         <v>38</v>
@@ -12536,33 +12536,33 @@
         <v>1</v>
       </c>
       <c r="E69">
-        <v>9.5139999999999993</v>
+        <v>9.6110000000000007</v>
       </c>
       <c r="F69">
-        <v>2.794</v>
+        <v>2.7109999999999999</v>
       </c>
       <c r="G69">
-        <v>1.555E-2</v>
+        <v>1.5440000000000001E-2</v>
       </c>
       <c r="H69">
-        <v>0.19159999999999999</v>
+        <v>0.18590000000000001</v>
       </c>
       <c r="I69">
-        <v>0.1628</v>
+        <v>0.15790000000000001</v>
       </c>
       <c r="J69">
-        <v>6.6379999999999999</v>
+        <v>6.6239999999999997</v>
       </c>
       <c r="K69">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>14</v>
       </c>
       <c r="B70" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C70" t="s">
         <v>38</v>
@@ -12574,19 +12574,19 @@
         <v>9.6110000000000007</v>
       </c>
       <c r="F70">
-        <v>2.7109999999999999</v>
+        <v>2.7170000000000001</v>
       </c>
       <c r="G70">
-        <v>1.5440000000000001E-2</v>
+        <v>1.6039999999999999E-2</v>
       </c>
       <c r="H70">
-        <v>0.18590000000000001</v>
+        <v>0.184</v>
       </c>
       <c r="I70">
-        <v>0.15790000000000001</v>
+        <v>0.15590000000000001</v>
       </c>
       <c r="J70">
-        <v>6.6239999999999997</v>
+        <v>6.54</v>
       </c>
       <c r="K70">
         <v>29</v>
@@ -12627,12 +12627,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>14</v>
       </c>
       <c r="B72" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C72" t="s">
         <v>38</v>
@@ -12641,25 +12641,25 @@
         <v>1</v>
       </c>
       <c r="E72">
-        <v>9.6110000000000007</v>
+        <v>8.7379999999999995</v>
       </c>
       <c r="F72">
-        <v>2.7170000000000001</v>
+        <v>2.6739999999999999</v>
       </c>
       <c r="G72">
-        <v>1.6039999999999999E-2</v>
+        <v>5.7329999999999999E-2</v>
       </c>
       <c r="H72">
-        <v>0.184</v>
+        <v>0.18640000000000001</v>
       </c>
       <c r="I72">
-        <v>0.15590000000000001</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="J72">
-        <v>6.54</v>
+        <v>4.1230000000000002</v>
       </c>
       <c r="K72">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -12697,74 +12697,74 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>14</v>
       </c>
       <c r="B74" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C74" t="s">
         <v>38</v>
       </c>
       <c r="D74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E74">
-        <v>8.7379999999999995</v>
+        <v>8.657</v>
       </c>
       <c r="F74">
-        <v>2.6739999999999999</v>
+        <v>2.9729999999999999</v>
       </c>
       <c r="G74">
-        <v>5.7329999999999999E-2</v>
+        <v>6.5759999999999999E-2</v>
       </c>
       <c r="H74">
-        <v>0.18640000000000001</v>
+        <v>0.18529999999999999</v>
       </c>
       <c r="I74">
-        <v>0.14119999999999999</v>
+        <v>0.13739999999999999</v>
       </c>
       <c r="J74">
-        <v>4.1230000000000002</v>
+        <v>3.8679999999999999</v>
       </c>
       <c r="K74">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>14</v>
       </c>
       <c r="B75" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C75" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="D75">
         <v>0</v>
       </c>
       <c r="E75">
-        <v>8.657</v>
+        <v>15.357200000000001</v>
       </c>
       <c r="F75">
-        <v>2.9729999999999999</v>
+        <v>-0.7712</v>
       </c>
       <c r="G75">
-        <v>6.5759999999999999E-2</v>
+        <v>2.4799999999999999E-2</v>
       </c>
       <c r="H75">
-        <v>0.18529999999999999</v>
+        <v>0.1358</v>
       </c>
       <c r="I75">
-        <v>0.13739999999999999</v>
+        <v>0.1111</v>
       </c>
       <c r="J75">
-        <v>3.8679999999999999</v>
+        <v>5.5010000000000003</v>
       </c>
       <c r="K75">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -12837,7 +12837,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>24</v>
       </c>
@@ -13047,7 +13047,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>24</v>
       </c>
@@ -13292,7 +13292,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>24</v>
       </c>
@@ -13537,74 +13537,74 @@
         <v>37</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>14</v>
       </c>
       <c r="B98" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C98" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="D98">
         <v>0</v>
       </c>
       <c r="E98">
-        <v>9.4819999999999993</v>
+        <v>13.866199999999999</v>
       </c>
       <c r="F98">
-        <v>2.081</v>
+        <v>-0.55179999999999996</v>
       </c>
       <c r="G98">
-        <v>9.6430000000000002E-2</v>
+        <v>5.4879999999999998E-2</v>
       </c>
       <c r="H98">
-        <v>9.9000000000000005E-2</v>
+        <v>0.1013</v>
       </c>
       <c r="I98">
-        <v>6.5629999999999994E-2</v>
+        <v>7.5630000000000003E-2</v>
       </c>
       <c r="J98">
-        <v>2.9670000000000001</v>
+        <v>3.9449999999999998</v>
       </c>
       <c r="K98">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>14</v>
       </c>
       <c r="B99" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C99" t="s">
         <v>55</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E99">
-        <v>15.357200000000001</v>
+        <v>-0.81950000000000001</v>
       </c>
       <c r="F99">
-        <v>-0.7712</v>
+        <v>2.7115999999999998</v>
       </c>
       <c r="G99">
-        <v>2.4799999999999999E-2</v>
+        <v>5.2560000000000003E-2</v>
       </c>
       <c r="H99">
-        <v>0.1358</v>
+        <v>9.7820000000000004E-2</v>
       </c>
       <c r="I99">
-        <v>0.1111</v>
+        <v>7.3429999999999995E-2</v>
       </c>
       <c r="J99">
-        <v>5.5010000000000003</v>
+        <v>4.0119999999999996</v>
       </c>
       <c r="K99">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -13887,47 +13887,47 @@
         <v>36</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>14</v>
       </c>
       <c r="B108" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C108" t="s">
         <v>55</v>
       </c>
       <c r="D108">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E108">
-        <v>13.866199999999999</v>
+        <v>4.0232999999999999</v>
       </c>
       <c r="F108">
-        <v>-0.55179999999999996</v>
+        <v>0.32650000000000001</v>
       </c>
       <c r="G108">
-        <v>5.4879999999999998E-2</v>
+        <v>5.3269999999999998E-2</v>
       </c>
       <c r="H108">
-        <v>0.1013</v>
+        <v>9.7259999999999999E-2</v>
       </c>
       <c r="I108">
-        <v>7.5630000000000003E-2</v>
+        <v>7.2859999999999994E-2</v>
       </c>
       <c r="J108">
-        <v>3.9449999999999998</v>
+        <v>3.9860000000000002</v>
       </c>
       <c r="K108">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>14</v>
       </c>
       <c r="B109" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C109" t="s">
         <v>55</v>
@@ -13936,68 +13936,68 @@
         <v>2</v>
       </c>
       <c r="E109">
-        <v>-0.81950000000000001</v>
+        <v>-0.38350000000000001</v>
       </c>
       <c r="F109">
-        <v>2.7115999999999998</v>
+        <v>0.21790000000000001</v>
       </c>
       <c r="G109">
-        <v>5.2560000000000003E-2</v>
+        <v>5.7689999999999998E-2</v>
       </c>
       <c r="H109">
-        <v>9.7820000000000004E-2</v>
+        <v>9.3969999999999998E-2</v>
       </c>
       <c r="I109">
-        <v>7.3429999999999995E-2</v>
+        <v>6.948E-2</v>
       </c>
       <c r="J109">
-        <v>4.0119999999999996</v>
+        <v>3.8370000000000002</v>
       </c>
       <c r="K109">
         <v>37</v>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>14</v>
       </c>
       <c r="B110" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C110" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D110">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E110">
-        <v>4.0232999999999999</v>
+        <v>9.4819999999999993</v>
       </c>
       <c r="F110">
-        <v>0.32650000000000001</v>
+        <v>2.081</v>
       </c>
       <c r="G110">
-        <v>5.3269999999999998E-2</v>
+        <v>9.6430000000000002E-2</v>
       </c>
       <c r="H110">
-        <v>9.7259999999999999E-2</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="I110">
-        <v>7.2859999999999994E-2</v>
+        <v>6.5629999999999994E-2</v>
       </c>
       <c r="J110">
-        <v>3.9860000000000002</v>
+        <v>2.9670000000000001</v>
       </c>
       <c r="K110">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>14</v>
       </c>
       <c r="B111" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C111" t="s">
         <v>55</v>
@@ -14006,60 +14006,60 @@
         <v>2</v>
       </c>
       <c r="E111">
-        <v>-0.38350000000000001</v>
+        <v>5.2873999999999999</v>
       </c>
       <c r="F111">
-        <v>0.21790000000000001</v>
+        <v>0.34339999999999998</v>
       </c>
       <c r="G111">
-        <v>5.7689999999999998E-2</v>
+        <v>6.7089999999999997E-2</v>
       </c>
       <c r="H111">
-        <v>9.3969999999999998E-2</v>
+        <v>8.7749999999999995E-2</v>
       </c>
       <c r="I111">
-        <v>6.948E-2</v>
+        <v>6.3100000000000003E-2</v>
       </c>
       <c r="J111">
-        <v>3.8370000000000002</v>
+        <v>3.5590000000000002</v>
       </c>
       <c r="K111">
         <v>37</v>
       </c>
     </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>14</v>
       </c>
       <c r="B112" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C112" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D112">
         <v>2</v>
       </c>
       <c r="E112">
-        <v>5.2873999999999999</v>
+        <v>-35.856999999999999</v>
       </c>
       <c r="F112">
-        <v>0.34339999999999998</v>
+        <v>2.2240000000000002</v>
       </c>
       <c r="G112">
-        <v>6.7089999999999997E-2</v>
+        <v>7.2859999999999994E-2</v>
       </c>
       <c r="H112">
-        <v>8.7749999999999995E-2</v>
+        <v>8.9020000000000002E-2</v>
       </c>
       <c r="I112">
-        <v>6.3100000000000003E-2</v>
+        <v>6.2990000000000004E-2</v>
       </c>
       <c r="J112">
-        <v>3.5590000000000002</v>
+        <v>3.42</v>
       </c>
       <c r="K112">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -14486,10 +14486,10 @@
   <autoFilter ref="A1:K124" xr:uid="{49AE83B7-BE4F-43DA-873C-DBE3365449F6}">
     <filterColumn colId="0">
       <filters>
-        <filter val="B90_MatureFemaleCPUE"/>
+        <filter val="B90_CPUE"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:K91">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:K112">
       <sortCondition descending="1" ref="I2:I124"/>
     </sortState>
   </autoFilter>
@@ -20873,10 +20873,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5650F765-A6D9-48FC-BD7C-177AA913FACD}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A5" sqref="A2:I163"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G37" sqref="A6:G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20917,7 +20918,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -20940,7 +20941,7 @@
         <v>0.51300000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -20963,7 +20964,7 @@
         <v>0.51200000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -20986,7 +20987,7 @@
         <v>0.4869</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -21032,7 +21033,7 @@
         <v>0.48180000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -21055,7 +21056,7 @@
         <v>0.45910000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -21078,7 +21079,7 @@
         <v>0.45710000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>112</v>
       </c>
@@ -21101,7 +21102,7 @@
         <v>0.44850000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -21124,7 +21125,7 @@
         <v>0.43719999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -21147,7 +21148,7 @@
         <v>0.43169999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -21170,7 +21171,7 @@
         <v>0.42330000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>112</v>
       </c>
@@ -21193,7 +21194,7 @@
         <v>0.41420000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>112</v>
       </c>
@@ -21216,7 +21217,7 @@
         <v>0.41299999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>112</v>
       </c>
@@ -21239,7 +21240,7 @@
         <v>0.40910000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -21262,7 +21263,7 @@
         <v>0.40039999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -21285,7 +21286,7 @@
         <v>0.39600000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>112</v>
       </c>
@@ -21308,7 +21309,7 @@
         <v>0.39400000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -21331,7 +21332,7 @@
         <v>0.39300000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -21354,7 +21355,7 @@
         <v>0.3876</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>112</v>
       </c>
@@ -21377,7 +21378,7 @@
         <v>0.38690000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -21423,7 +21424,7 @@
         <v>0.37969999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>83</v>
       </c>
@@ -21446,7 +21447,7 @@
         <v>0.37859999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -21469,7 +21470,7 @@
         <v>0.3745</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>83</v>
       </c>
@@ -21515,7 +21516,7 @@
         <v>0.35720000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -21538,7 +21539,7 @@
         <v>0.35720000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -21561,7 +21562,7 @@
         <v>0.35670000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -21584,7 +21585,7 @@
         <v>0.3523</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -21607,7 +21608,7 @@
         <v>0.34739999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -21630,7 +21631,7 @@
         <v>0.34720000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -21653,7 +21654,7 @@
         <v>0.33779999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>121</v>
       </c>
@@ -21676,7 +21677,7 @@
         <v>0.33689999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -21699,7 +21700,7 @@
         <v>0.3362</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -21745,7 +21746,7 @@
         <v>0.33069999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -21768,7 +21769,7 @@
         <v>0.32869999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -21791,7 +21792,7 @@
         <v>0.32790000000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -21814,7 +21815,7 @@
         <v>0.32769999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>112</v>
       </c>
@@ -21837,7 +21838,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>29</v>
       </c>
@@ -21860,7 +21861,7 @@
         <v>0.31950000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -21883,7 +21884,7 @@
         <v>0.31209999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>20</v>
       </c>
@@ -21906,7 +21907,7 @@
         <v>0.31019999999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>121</v>
       </c>
@@ -21929,7 +21930,7 @@
         <v>0.30959999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>20</v>
       </c>
@@ -21952,7 +21953,7 @@
         <v>0.30859999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>28</v>
       </c>
@@ -21975,7 +21976,7 @@
         <v>0.3044</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>29</v>
       </c>
@@ -21998,7 +21999,7 @@
         <v>0.30349999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>22</v>
       </c>
@@ -22044,7 +22045,7 @@
         <v>0.30109999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>112</v>
       </c>
@@ -22067,7 +22068,7 @@
         <v>0.30080000000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>20</v>
       </c>
@@ -22090,7 +22091,7 @@
         <v>0.30009999999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>29</v>
       </c>
@@ -22136,7 +22137,7 @@
         <v>0.29239999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>83</v>
       </c>
@@ -22159,7 +22160,7 @@
         <v>0.29170000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>83</v>
       </c>
@@ -22182,7 +22183,7 @@
         <v>0.29060000000000002</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>112</v>
       </c>
@@ -22205,7 +22206,7 @@
         <v>0.28820000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>83</v>
       </c>
@@ -22228,7 +22229,7 @@
         <v>0.28670000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>20</v>
       </c>
@@ -22251,7 +22252,7 @@
         <v>0.28649999999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>83</v>
       </c>
@@ -22297,7 +22298,7 @@
         <v>0.28399999999999997</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>22</v>
       </c>
@@ -22343,7 +22344,7 @@
         <v>0.28370000000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>121</v>
       </c>
@@ -22366,7 +22367,7 @@
         <v>0.28239999999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>29</v>
       </c>
@@ -22389,7 +22390,7 @@
         <v>0.28120000000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>22</v>
       </c>
@@ -22435,7 +22436,7 @@
         <v>0.28050000000000003</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>112</v>
       </c>
@@ -22481,7 +22482,7 @@
         <v>0.27639999999999998</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>83</v>
       </c>
@@ -22504,7 +22505,7 @@
         <v>0.27410000000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>22</v>
       </c>
@@ -22550,7 +22551,7 @@
         <v>0.27379999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>112</v>
       </c>
@@ -22573,7 +22574,7 @@
         <v>0.27289999999999998</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>29</v>
       </c>
@@ -22596,7 +22597,7 @@
         <v>0.26579999999999998</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>20</v>
       </c>
@@ -22619,7 +22620,7 @@
         <v>0.2636</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>19</v>
       </c>
@@ -22642,7 +22643,7 @@
         <v>0.26169999999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>28</v>
       </c>
@@ -22665,7 +22666,7 @@
         <v>0.2576</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>22</v>
       </c>
@@ -22711,7 +22712,7 @@
         <v>0.25559999999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>22</v>
       </c>
@@ -22757,7 +22758,7 @@
         <v>0.25440000000000002</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>28</v>
       </c>
@@ -22780,7 +22781,7 @@
         <v>0.25390000000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>28</v>
       </c>
@@ -22803,7 +22804,7 @@
         <v>0.25080000000000002</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>112</v>
       </c>
@@ -22826,7 +22827,7 @@
         <v>0.24809999999999999</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>28</v>
       </c>
@@ -22849,7 +22850,7 @@
         <v>0.24640000000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>22</v>
       </c>
@@ -22895,7 +22896,7 @@
         <v>0.24390000000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>28</v>
       </c>
@@ -22941,7 +22942,7 @@
         <v>0.24229999999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>83</v>
       </c>
@@ -22964,7 +22965,7 @@
         <v>0.2412</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>83</v>
       </c>
@@ -22987,7 +22988,7 @@
         <v>0.23830000000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>22</v>
       </c>
@@ -23033,7 +23034,7 @@
         <v>0.23749999999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>28</v>
       </c>
@@ -23056,7 +23057,7 @@
         <v>0.23580000000000001</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>112</v>
       </c>
@@ -23079,7 +23080,7 @@
         <v>0.23430000000000001</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>121</v>
       </c>
@@ -23102,7 +23103,7 @@
         <v>0.2339</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>30</v>
       </c>
@@ -23125,7 +23126,7 @@
         <v>0.2334</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>112</v>
       </c>
@@ -23148,7 +23149,7 @@
         <v>0.23150000000000001</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>28</v>
       </c>
@@ -23171,7 +23172,7 @@
         <v>0.23089999999999999</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>29</v>
       </c>
@@ -23194,7 +23195,7 @@
         <v>0.23039999999999999</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>28</v>
       </c>
@@ -23217,7 +23218,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>28</v>
       </c>
@@ -23240,7 +23241,7 @@
         <v>0.2298</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>20</v>
       </c>
@@ -23263,7 +23264,7 @@
         <v>0.2283</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>22</v>
       </c>
@@ -23309,7 +23310,7 @@
         <v>0.22789999999999999</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>30</v>
       </c>
@@ -23332,7 +23333,7 @@
         <v>0.22770000000000001</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>83</v>
       </c>
@@ -23355,7 +23356,7 @@
         <v>0.22670000000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>121</v>
       </c>
@@ -23378,7 +23379,7 @@
         <v>0.2261</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>121</v>
       </c>
@@ -23401,7 +23402,7 @@
         <v>0.22489999999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>83</v>
       </c>
@@ -23424,7 +23425,7 @@
         <v>0.2243</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>83</v>
       </c>
@@ -23447,7 +23448,7 @@
         <v>0.22389999999999999</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>28</v>
       </c>
@@ -23470,7 +23471,7 @@
         <v>0.2238</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>28</v>
       </c>
@@ -23493,7 +23494,7 @@
         <v>0.2235</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>20</v>
       </c>
@@ -23539,7 +23540,7 @@
         <v>0.2228</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>20</v>
       </c>
@@ -23562,7 +23563,7 @@
         <v>0.22209999999999999</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>30</v>
       </c>
@@ -23585,7 +23586,7 @@
         <v>0.2218</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>30</v>
       </c>
@@ -23608,7 +23609,7 @@
         <v>0.2167</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>28</v>
       </c>
@@ -23631,7 +23632,7 @@
         <v>0.21659999999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>112</v>
       </c>
@@ -23654,7 +23655,7 @@
         <v>0.21340000000000001</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>28</v>
       </c>
@@ -23677,7 +23678,7 @@
         <v>0.21290000000000001</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>30</v>
       </c>
@@ -23700,7 +23701,7 @@
         <v>0.21260000000000001</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>28</v>
       </c>
@@ -23723,7 +23724,7 @@
         <v>0.21179999999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>112</v>
       </c>
@@ -23769,7 +23770,7 @@
         <v>0.20549999999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>112</v>
       </c>
@@ -23792,7 +23793,7 @@
         <v>0.2039</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>29</v>
       </c>
@@ -23815,7 +23816,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>20</v>
       </c>
@@ -23838,7 +23839,7 @@
         <v>0.20250000000000001</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>30</v>
       </c>
@@ -23861,7 +23862,7 @@
         <v>0.2024</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>22</v>
       </c>
@@ -23907,7 +23908,7 @@
         <v>0.20200000000000001</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>30</v>
       </c>
@@ -23930,7 +23931,7 @@
         <v>0.20119999999999999</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>30</v>
       </c>
@@ -23953,7 +23954,7 @@
         <v>0.19980000000000001</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>30</v>
       </c>
@@ -23976,7 +23977,7 @@
         <v>0.1993</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>121</v>
       </c>
@@ -23999,7 +24000,7 @@
         <v>0.19589999999999999</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>30</v>
       </c>
@@ -24022,7 +24023,7 @@
         <v>0.1928</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>112</v>
       </c>
@@ -24045,7 +24046,7 @@
         <v>0.18940000000000001</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>112</v>
       </c>
@@ -24068,7 +24069,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>28</v>
       </c>
@@ -24114,7 +24115,7 @@
         <v>0.18049999999999999</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>112</v>
       </c>
@@ -24137,7 +24138,7 @@
         <v>0.17860000000000001</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>29</v>
       </c>
@@ -24206,7 +24207,7 @@
         <v>0.16020000000000001</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>33</v>
       </c>
@@ -24229,7 +24230,7 @@
         <v>0.15040000000000001</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>29</v>
       </c>
@@ -24275,7 +24276,7 @@
         <v>0.14269999999999999</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>33</v>
       </c>
@@ -24298,7 +24299,7 @@
         <v>0.1389</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>29</v>
       </c>
@@ -24344,7 +24345,7 @@
         <v>0.1265</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>29</v>
       </c>
@@ -24367,7 +24368,7 @@
         <v>0.1227</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>33</v>
       </c>
@@ -24390,7 +24391,7 @@
         <v>0.1187</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>19</v>
       </c>
@@ -24413,7 +24414,7 @@
         <v>0.1158</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>19</v>
       </c>
@@ -24436,7 +24437,7 @@
         <v>0.1132</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>19</v>
       </c>
@@ -24459,7 +24460,7 @@
         <v>0.10009999999999999</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>29</v>
       </c>
@@ -24482,7 +24483,7 @@
         <v>9.6939999999999998E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>29</v>
       </c>
@@ -24505,7 +24506,7 @@
         <v>9.5610000000000001E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>19</v>
       </c>
@@ -24574,7 +24575,7 @@
         <v>7.6590000000000005E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>19</v>
       </c>
@@ -24597,7 +24598,7 @@
         <v>7.2830000000000006E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>33</v>
       </c>
@@ -24620,7 +24621,7 @@
         <v>6.1420000000000002E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>29</v>
       </c>
@@ -24645,6 +24646,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I163" xr:uid="{CC90FC41-3066-4941-A442-653857C60AC5}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="MeanLandings"/>
+        <filter val="MeanLandingsCPUE"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I163">
       <sortCondition descending="1" ref="G2:G163"/>
     </sortState>

</xml_diff>

<commit_message>
Finished analyses for Kendrick mtg 2019-08-26
</commit_message>
<xml_diff>
--- a/regression_summaries.xlsx
+++ b/regression_summaries.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sczwa\Desktop\shinycrab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\shinycrab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C24D3E6-D7FA-423E-A9A5-2972410B4BBA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324741A0-D1CD-4971-9CCA-E49D3FE734B2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4095" windowWidth="24240" windowHeight="13140" firstSheet="1" activeTab="3" xr2:uid="{92501DCD-C878-4E1C-B363-916EF62D2436}"/>
+    <workbookView xWindow="-19320" yWindow="270" windowWidth="19440" windowHeight="15000" firstSheet="1" activeTab="6" xr2:uid="{92501DCD-C878-4E1C-B363-916EF62D2436}"/>
   </bookViews>
   <sheets>
     <sheet name="E98" sheetId="2" r:id="rId1"/>
@@ -10128,7 +10128,7 @@
   </sheetPr>
   <dimension ref="A1:K124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD14"/>
     </sheetView>
@@ -16638,7 +16638,7 @@
   <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18637,12 +18637,13 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.5703125" customWidth="1"/>
     <col min="4" max="8" width="15.28515625" customWidth="1"/>
   </cols>
@@ -18673,7 +18674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -18793,7 +18794,7 @@
         <v>0.40489999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -18933,7 +18934,7 @@
         <v>0.31940000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -19053,7 +19054,7 @@
         <v>0.2989</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -19093,7 +19094,7 @@
         <v>0.29820000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -19193,7 +19194,7 @@
         <v>0.27110000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -19253,7 +19254,7 @@
         <v>0.26640000000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -19293,7 +19294,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -19333,7 +19334,7 @@
         <v>0.25440000000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -19373,7 +19374,7 @@
         <v>0.25290000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -19413,7 +19414,7 @@
         <v>0.246</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>34</v>
       </c>
@@ -19493,7 +19494,7 @@
         <v>0.22839999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>23</v>
       </c>
@@ -19513,7 +19514,7 @@
         <v>0.22839999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>34</v>
       </c>
@@ -19573,7 +19574,7 @@
         <v>0.22670000000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>23</v>
       </c>
@@ -19613,7 +19614,7 @@
         <v>0.22420000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>34</v>
       </c>
@@ -19633,7 +19634,7 @@
         <v>0.22420000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>83</v>
       </c>
@@ -19693,7 +19694,7 @@
         <v>0.21840000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>34</v>
       </c>
@@ -19753,7 +19754,7 @@
         <v>0.21229999999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>83</v>
       </c>
@@ -19813,7 +19814,7 @@
         <v>0.2046</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>34</v>
       </c>
@@ -19873,7 +19874,7 @@
         <v>0.19309999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>34</v>
       </c>
@@ -19933,7 +19934,7 @@
         <v>0.17519999999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>34</v>
       </c>
@@ -19953,7 +19954,7 @@
         <v>0.17480000000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>34</v>
       </c>
@@ -20113,7 +20114,7 @@
         <v>0.15260000000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>34</v>
       </c>
@@ -20173,7 +20174,7 @@
         <v>0.14430000000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>34</v>
       </c>
@@ -20213,7 +20214,7 @@
         <v>0.12670000000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>34</v>
       </c>
@@ -20253,7 +20254,7 @@
         <v>0.1118</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>34</v>
       </c>
@@ -20453,7 +20454,7 @@
         <v>9.4990000000000005E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>34</v>
       </c>
@@ -20513,7 +20514,7 @@
         <v>8.6499999999999994E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>34</v>
       </c>
@@ -20553,7 +20554,7 @@
         <v>8.5639999999999994E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>34</v>
       </c>
@@ -20613,7 +20614,7 @@
         <v>8.3680000000000004E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>34</v>
       </c>
@@ -20693,7 +20694,7 @@
         <v>7.689E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>34</v>
       </c>
@@ -20713,7 +20714,7 @@
         <v>7.6369999999999993E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>34</v>
       </c>
@@ -20833,7 +20834,7 @@
         <v>7.0180000000000006E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>34</v>
       </c>
@@ -20857,7 +20858,8 @@
   <autoFilter ref="A1:H110" xr:uid="{663E3F2F-6B72-4B60-89F8-B414401CFF8F}">
     <filterColumn colId="0">
       <filters>
-        <filter val="AshleyLandingsCPUE"/>
+        <filter val="MeanLandings"/>
+        <filter val="MeanLandingsCPUE"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H110">

</xml_diff>